<commit_message>
Final update: all measurement files saved
</commit_message>
<xml_diff>
--- a/metadata_sponge.xlsx
+++ b/metadata_sponge.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aneeshbondugula/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aneeshbondugula/Downloads/lolsort/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD9E168-3A98-4E47-ACE2-6EB5EE5CB1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34616660-0A3F-9B4E-A0CB-FC7ABA363E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17060" activeTab="82" xr2:uid="{261E118F-B2D0-4B12-8586-BA9BCD61FB2E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17020" xr2:uid="{261E118F-B2D0-4B12-8586-BA9BCD61FB2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorted Slides List" sheetId="23" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2938" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="439">
   <si>
     <t>S/N</t>
   </si>
@@ -1435,6 +1435,9 @@
   </si>
   <si>
     <t>many raphide bundles</t>
+  </si>
+  <si>
+    <t>ZRC.POR.634</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2131,8 @@
   </sheetPr>
   <dimension ref="A1:L675"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H475" sqref="H475:H496"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13305,7 +13308,9 @@
       <c r="G475" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H475" s="42"/>
+      <c r="H475" s="42" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="476" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A476" s="6">
@@ -20990,7 +20995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0484027-6E7D-4F49-9100-FC726238BA9E}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>

</xml_diff>